<commit_message>
Update Total Address Growth Rate, simplified line plot.xlsx
</commit_message>
<xml_diff>
--- a/Output/Total Address Growth Rate, simplified line plot.xlsx
+++ b/Output/Total Address Growth Rate, simplified line plot.xlsx
@@ -398,10 +398,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>0.685081917733825</v>
+        <v>0.69702201161685</v>
       </c>
       <c r="C2" t="n">
-        <v>0.948552807859175</v>
+        <v>0.959540820537664</v>
       </c>
     </row>
     <row r="3">
@@ -409,10 +409,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>0.635486880163547</v>
+        <v>0.666701849462522</v>
       </c>
       <c r="C3" t="n">
-        <v>0.940670004141592</v>
+        <v>0.957008406613708</v>
       </c>
     </row>
     <row r="4">
@@ -420,10 +420,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>0.64658968838295</v>
+        <v>0.583992829750318</v>
       </c>
       <c r="C4" t="n">
-        <v>0.984348362176356</v>
+        <v>0.966332181041396</v>
       </c>
     </row>
     <row r="5">
@@ -431,10 +431,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>0.743462845124865</v>
+        <v>0.742867022606371</v>
       </c>
       <c r="C5" t="n">
-        <v>1.03880402256979</v>
+        <v>1.04756605954615</v>
       </c>
     </row>
     <row r="6">
@@ -442,10 +442,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>0.774767892976828</v>
+        <v>0.853251012486298</v>
       </c>
       <c r="C6" t="n">
-        <v>1.0756984249381</v>
+        <v>1.10302645401185</v>
       </c>
     </row>
     <row r="7">
@@ -453,10 +453,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="n">
-        <v>0.731584676456879</v>
+        <v>0.720324947983116</v>
       </c>
       <c r="C7" t="n">
-        <v>1.00386156191104</v>
+        <v>1.01493040177363</v>
       </c>
     </row>
     <row r="8">
@@ -464,10 +464,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="n">
-        <v>0.995269587743164</v>
+        <v>1.07780490606319</v>
       </c>
       <c r="C8" t="n">
-        <v>1.18120937604043</v>
+        <v>1.1993541509557</v>
       </c>
     </row>
     <row r="9">
@@ -475,10 +475,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="n">
-        <v>1.25194831445207</v>
+        <v>1.25423446391663</v>
       </c>
       <c r="C9" t="n">
-        <v>1.24144636667135</v>
+        <v>1.22209793398939</v>
       </c>
     </row>
     <row r="10">
@@ -486,10 +486,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>1.03817325150731</v>
+        <v>1.05719642346785</v>
       </c>
       <c r="C10" t="n">
-        <v>0.97915871402117</v>
+        <v>1.03408641106742</v>
       </c>
     </row>
     <row r="11">
@@ -497,10 +497,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>1.82072911431817</v>
+        <v>1.72977297960731</v>
       </c>
       <c r="C11" t="n">
-        <v>1.46551514537763</v>
+        <v>1.36114709035375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>